<commit_message>
updated erm and tableview
</commit_message>
<xml_diff>
--- a/DB/DB-Tabellen.xlsx
+++ b/DB/DB-Tabellen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.pucher\OneDrive - HTL Vöcklabruck\5AHWII\SWP\MensaBestellung\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{30733CB3-82C6-487A-BAEC-0BCFD25EFE75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="6_{30733CB3-82C6-487A-BAEC-0BCFD25EFE75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8894C54D-D06E-4537-A5F1-6C705EE6A305}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{69F0ACEA-CC57-4D04-AAC5-5D1233FB1C87}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>User</t>
   </si>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868B0A42-807B-4D03-843A-C7C4AC5180CF}">
   <dimension ref="A2:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,6 +608,9 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
@@ -637,6 +640,9 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
@@ -657,6 +663,9 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
@@ -688,6 +697,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B3F2DBAE4AB154BA9BC4F40229DE4C2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="298a960356b0bb5c4bf5db6d01e10e10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a2675265-d0c3-4a9e-a2cd-bad11ce77d07" xmlns:ns4="84c3105f-dc73-429a-a1bf-d7709250548d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cf9d9dd511bd04a96fbcc7f654d3f3cb" ns3:_="" ns4:_="">
     <xsd:import namespace="a2675265-d0c3-4a9e-a2cd-bad11ce77d07"/>
@@ -910,22 +934,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B6EB97-4373-4077-ADAA-CB59ACE759CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="84c3105f-dc73-429a-a1bf-d7709250548d"/>
+    <ds:schemaRef ds:uri="a2675265-d0c3-4a9e-a2cd-bad11ce77d07"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC2B00E-AFC6-4FD4-9175-8D30CFE0307C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{405D245C-15FD-4A2B-A932-E9C1A4B734AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -942,29 +976,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC2B00E-AFC6-4FD4-9175-8D30CFE0307C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B6EB97-4373-4077-ADAA-CB59ACE759CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a2675265-d0c3-4a9e-a2cd-bad11ce77d07"/>
-    <ds:schemaRef ds:uri="84c3105f-dc73-429a-a1bf-d7709250548d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
db filled & update
da filled with test data and minor design changes
</commit_message>
<xml_diff>
--- a/DB/DB-Tabellen.xlsx
+++ b/DB/DB-Tabellen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.pucher\OneDrive - HTL Vöcklabruck\5AHWII\SWP\MensaBestellung\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="6_{30733CB3-82C6-487A-BAEC-0BCFD25EFE75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{DE24947F-2F8C-430D-AB42-C3C2CF8CC27F}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="6_{30733CB3-82C6-487A-BAEC-0BCFD25EFE75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{930A097C-9974-460B-B67F-C84FC2E01B5B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{69F0ACEA-CC57-4D04-AAC5-5D1233FB1C87}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>description</t>
   </si>
   <si>
-    <t>isActive</t>
+    <t>mensaOpen</t>
   </si>
 </sst>
 </file>
@@ -501,11 +501,12 @@
   <dimension ref="A2:W7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="19.42578125" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
@@ -706,6 +707,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B3F2DBAE4AB154BA9BC4F40229DE4C2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="298a960356b0bb5c4bf5db6d01e10e10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a2675265-d0c3-4a9e-a2cd-bad11ce77d07" xmlns:ns4="84c3105f-dc73-429a-a1bf-d7709250548d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cf9d9dd511bd04a96fbcc7f654d3f3cb" ns3:_="" ns4:_="">
     <xsd:import namespace="a2675265-d0c3-4a9e-a2cd-bad11ce77d07"/>
@@ -928,22 +944,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B6EB97-4373-4077-ADAA-CB59ACE759CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a2675265-d0c3-4a9e-a2cd-bad11ce77d07"/>
+    <ds:schemaRef ds:uri="84c3105f-dc73-429a-a1bf-d7709250548d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC2B00E-AFC6-4FD4-9175-8D30CFE0307C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{405D245C-15FD-4A2B-A932-E9C1A4B734AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -960,29 +986,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC2B00E-AFC6-4FD4-9175-8D30CFE0307C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B6EB97-4373-4077-ADAA-CB59ACE759CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="84c3105f-dc73-429a-a1bf-d7709250548d"/>
-    <ds:schemaRef ds:uri="a2675265-d0c3-4a9e-a2cd-bad11ce77d07"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
db functionality & methods
changed db, added project functions and localised resources
</commit_message>
<xml_diff>
--- a/DB/DB-Tabellen.xlsx
+++ b/DB/DB-Tabellen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.pucher\OneDrive - HTL Vöcklabruck\5AHWII\SWP\MensaBestellung\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="6_{30733CB3-82C6-487A-BAEC-0BCFD25EFE75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{930A097C-9974-460B-B67F-C84FC2E01B5B}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="14_{B7C0E6C4-A7F1-42A6-B51D-1974FBDCD2F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{05606128-0961-4750-AF4B-34E990319309}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{69F0ACEA-CC57-4D04-AAC5-5D1233FB1C87}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>User</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>mensaOpen</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>foodExchangeOpen</t>
+  </si>
+  <si>
+    <t>datetime</t>
   </si>
 </sst>
 </file>
@@ -498,18 +510,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868B0A42-807B-4D03-843A-C7C4AC5180CF}">
-  <dimension ref="A2:W7"/>
+  <dimension ref="A2:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.42578125" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
     <col min="17" max="17" width="14.5703125" customWidth="1"/>
@@ -685,10 +698,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>7</v>
@@ -698,6 +711,22 @@
       </c>
       <c r="R7" s="6" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -947,15 +976,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B6EB97-4373-4077-ADAA-CB59ACE759CD}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="84c3105f-dc73-429a-a1bf-d7709250548d"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="a2675265-d0c3-4a9e-a2cd-bad11ce77d07"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a2675265-d0c3-4a9e-a2cd-bad11ce77d07"/>
-    <ds:schemaRef ds:uri="84c3105f-dc73-429a-a1bf-d7709250548d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>